<commit_message>
home page mobile mode
</commit_message>
<xml_diff>
--- a/0doc-things/popl - first page.xlsx
+++ b/0doc-things/popl - first page.xlsx
@@ -146,7 +146,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +156,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -172,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -191,6 +197,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1287,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1430,7 +1439,7 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="7" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="1">
@@ -1444,7 +1453,7 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="1">

</xml_diff>